<commit_message>
aggiornamento nome e dati del progetto
</commit_message>
<xml_diff>
--- a/Evaluacion.xlsx
+++ b/Evaluacion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanr\git\alg_PerezJuanRamonUO22223\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UO299008\git\alg_PanicoGianpietroUO299008\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,9 +37,6 @@
     <t>Prácticas 0, 1.1, 1.2 (Tiempos)</t>
   </si>
   <si>
-    <t>Pérez Pérez, Juan Ramón</t>
-  </si>
-  <si>
     <t>Práctica 2 (Ordenación)</t>
   </si>
   <si>
@@ -91,13 +88,16 @@
     <t>Columna7</t>
   </si>
   <si>
-    <t>UO22223@uniovi.es</t>
-  </si>
-  <si>
     <t>GitHub</t>
   </si>
   <si>
-    <t>https://github.com/juanrperez/alg_PerezJuanRamonUO22223</t>
+    <t>Gianpietro Panico</t>
+  </si>
+  <si>
+    <t>UO299008@uniovi.es</t>
+  </si>
+  <si>
+    <t>https://github.com/gianpietropanico/alg_PanicoGianpietroUO299008</t>
   </si>
 </sst>
 </file>
@@ -157,7 +157,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -194,11 +194,26 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -212,9 +227,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -230,15 +242,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -248,9 +265,6 @@
   </cellStyles>
   <dxfs count="20">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -509,6 +523,16 @@
           <color indexed="8"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -528,13 +552,6 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -549,26 +566,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla14515" displayName="Tabla14515" ref="A4:Q5" totalsRowShown="0" headerRowDxfId="18" dataDxfId="0" tableBorderDxfId="19">
-  <autoFilter ref="A4:Q5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla14515" displayName="Tabla14515" ref="A4:Q6" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" tableBorderDxfId="17">
+  <autoFilter ref="A4:Q6"/>
   <tableColumns count="17">
-    <tableColumn id="3" name="Estudiante" dataDxfId="17"/>
-    <tableColumn id="13" name="Prácticas 0, 1.1, 1.2 (Tiempos)" dataDxfId="16"/>
-    <tableColumn id="1" name="Columna1" dataDxfId="15"/>
-    <tableColumn id="14" name="Práctica 2 (Ordenación)" dataDxfId="14"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="13"/>
-    <tableColumn id="15" name="Práctica 3 (DV)" dataDxfId="12"/>
-    <tableColumn id="4" name="Columna3" dataDxfId="11"/>
-    <tableColumn id="16" name="Práctica 4 (Devorador)" dataDxfId="10"/>
-    <tableColumn id="5" name="Columna4" dataDxfId="9"/>
-    <tableColumn id="17" name="Práctica 5 (Prog. dinámica)" dataDxfId="8"/>
-    <tableColumn id="6" name="Columna5" dataDxfId="7"/>
-    <tableColumn id="18" name="Práctica 6 (Backtracking)" dataDxfId="6"/>
-    <tableColumn id="7" name="Columna6" dataDxfId="5"/>
-    <tableColumn id="19" name="Práctica 7 (Ramificación y poda)" dataDxfId="4"/>
-    <tableColumn id="8" name="Columna7" dataDxfId="3"/>
-    <tableColumn id="24" name="Control prácticas" dataDxfId="2"/>
-    <tableColumn id="21" name="Nota ev. Continua" dataDxfId="1"/>
+    <tableColumn id="3" name="Estudiante" dataDxfId="16"/>
+    <tableColumn id="13" name="Prácticas 0, 1.1, 1.2 (Tiempos)" dataDxfId="15"/>
+    <tableColumn id="1" name="Columna1" dataDxfId="14"/>
+    <tableColumn id="14" name="Práctica 2 (Ordenación)" dataDxfId="13"/>
+    <tableColumn id="2" name="Columna2" dataDxfId="12"/>
+    <tableColumn id="15" name="Práctica 3 (DV)" dataDxfId="11"/>
+    <tableColumn id="4" name="Columna3" dataDxfId="10"/>
+    <tableColumn id="16" name="Práctica 4 (Devorador)" dataDxfId="9"/>
+    <tableColumn id="5" name="Columna4" dataDxfId="8"/>
+    <tableColumn id="17" name="Práctica 5 (Prog. dinámica)" dataDxfId="7"/>
+    <tableColumn id="6" name="Columna5" dataDxfId="6"/>
+    <tableColumn id="18" name="Práctica 6 (Backtracking)" dataDxfId="5"/>
+    <tableColumn id="7" name="Columna6" dataDxfId="4"/>
+    <tableColumn id="19" name="Práctica 7 (Ramificación y poda)" dataDxfId="3"/>
+    <tableColumn id="8" name="Columna7" dataDxfId="2"/>
+    <tableColumn id="24" name="Control prácticas" dataDxfId="1"/>
+    <tableColumn id="21" name="Nota ev. Continua" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -864,414 +881,415 @@
   <dimension ref="A1:Q137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.26953125" customWidth="1"/>
-    <col min="2" max="2" width="26.453125" customWidth="1"/>
-    <col min="3" max="3" width="7.08984375" customWidth="1"/>
-    <col min="4" max="4" width="26.54296875" customWidth="1"/>
-    <col min="5" max="5" width="7.08984375" customWidth="1"/>
-    <col min="6" max="6" width="22.7265625" customWidth="1"/>
-    <col min="7" max="7" width="7.08984375" customWidth="1"/>
-    <col min="8" max="8" width="27.1796875" customWidth="1"/>
-    <col min="9" max="9" width="7.08984375" customWidth="1"/>
-    <col min="10" max="10" width="30.7265625" customWidth="1"/>
-    <col min="11" max="11" width="7.08984375" customWidth="1"/>
-    <col min="12" max="12" width="30.26953125" customWidth="1"/>
-    <col min="13" max="13" width="7.08984375" customWidth="1"/>
-    <col min="14" max="14" width="27.26953125" customWidth="1"/>
-    <col min="15" max="15" width="7.08984375" customWidth="1"/>
-    <col min="16" max="16" width="23.81640625" customWidth="1"/>
-    <col min="17" max="17" width="20.26953125" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" customWidth="1"/>
+    <col min="12" max="12" width="30.28515625" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" customWidth="1"/>
+    <col min="14" max="14" width="27.28515625" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" customWidth="1"/>
+    <col min="16" max="16" width="23.85546875" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="O3" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="D4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="I3" s="8">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0.13400000000000001</v>
-      </c>
-      <c r="M3" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="O3" s="7">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="13" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="N4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="O4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="P4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="Q4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="14"/>
+    </row>
+    <row r="7" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="11"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="11"/>
+    </row>
+    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-    </row>
-    <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="13"/>
-    </row>
-    <row r="7" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="14"/>
-    </row>
-    <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="14"/>
-    </row>
-    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="11"/>
+    </row>
+    <row r="9" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="14"/>
-    </row>
-    <row r="10" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="14"/>
-    </row>
-    <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="14"/>
-    </row>
-    <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="14"/>
-    </row>
-    <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="14"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="14"/>
-    </row>
-    <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="11"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="11"/>
+    </row>
+    <row r="10" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="11"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="11"/>
+    </row>
+    <row r="11" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="11"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="11"/>
+    </row>
+    <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="11"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="11"/>
+    </row>
+    <row r="13" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="11"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="11"/>
+    </row>
+    <row r="14" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio en MatrixOperacionesTiempos. Evaluación P0 y P11
</commit_message>
<xml_diff>
--- a/Evaluacion.xlsx
+++ b/Evaluacion.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UO299008\git\alg_PanicoGianpietroUO299008\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\git\alg_PanicoGianpietroUO299008\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,21 +15,11 @@
     <sheet name="Marks" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Estudiante</t>
   </si>
@@ -98,6 +88,28 @@
   </si>
   <si>
     <t>https://github.com/gianpietropanico/alg_PanicoGianpietroUO299008</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Los ficheros PDF de documentación se deben identificar al principio con el nombre y apellidos del estudiante y el grupo al que pertenece. P0.  Código correcto e incluye una clase para probar la funcionalidad -&gt; OK. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Hay un problema en los tiempos: los bucles de n y de repeticiones están bien, pero no sirven de nada si el tamaño de la matriz con la que trabajamos no es n (y siempre es 4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, he cambiado la de diagonal1() y he dejado la de diagonal2() como lo tenías para que veas la diferencia. P11. Suma y máximo OK, mide tiempo correctamente, uno &lt;50, pero los demás están correctos.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -107,10 +119,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -148,6 +167,30 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,7 +200,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -217,23 +260,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -242,13 +363,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -257,11 +378,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="63">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
+    <cellStyle name="Hipervínculo 2" xfId="3"/>
+    <cellStyle name="Hipervínculo 3" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="5"/>
+    <cellStyle name="Normal 3" xfId="6"/>
+    <cellStyle name="Normal 3 2" xfId="7"/>
+    <cellStyle name="Normal 3 3" xfId="8"/>
+    <cellStyle name="Normal 3 4" xfId="9"/>
+    <cellStyle name="Normal 3 4 2" xfId="10"/>
+    <cellStyle name="Normal 3 4 2 2" xfId="11"/>
+    <cellStyle name="Normal 3 4 3" xfId="12"/>
+    <cellStyle name="Normal 3 5" xfId="13"/>
+    <cellStyle name="Normal 3 5 2" xfId="14"/>
+    <cellStyle name="Normal 4" xfId="15"/>
+    <cellStyle name="Normal 4 2" xfId="16"/>
+    <cellStyle name="Normal 4 2 2" xfId="17"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="18"/>
+    <cellStyle name="Normal 4 2 2 2 2" xfId="19"/>
+    <cellStyle name="Normal 4 2 2 3" xfId="20"/>
+    <cellStyle name="Normal 4 2 3" xfId="21"/>
+    <cellStyle name="Normal 4 2 3 2" xfId="22"/>
+    <cellStyle name="Normal 4 2 4" xfId="23"/>
+    <cellStyle name="Normal 4 3" xfId="24"/>
+    <cellStyle name="Normal 4 3 2" xfId="25"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="26"/>
+    <cellStyle name="Normal 4 3 3" xfId="27"/>
+    <cellStyle name="Normal 4 3 3 2" xfId="28"/>
+    <cellStyle name="Normal 4 3 4" xfId="29"/>
+    <cellStyle name="Normal 4 4" xfId="30"/>
+    <cellStyle name="Normal 4 4 2" xfId="31"/>
+    <cellStyle name="Normal 4 4 2 2" xfId="32"/>
+    <cellStyle name="Normal 4 4 3" xfId="33"/>
+    <cellStyle name="Normal 4 5" xfId="34"/>
+    <cellStyle name="Normal 4 5 2" xfId="35"/>
+    <cellStyle name="Normal 4 6" xfId="36"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje 2" xfId="37"/>
+    <cellStyle name="Porcentaje 2 2" xfId="38"/>
+    <cellStyle name="Porcentaje 2 3" xfId="39"/>
+    <cellStyle name="Porcentaje 2 3 2" xfId="40"/>
+    <cellStyle name="Porcentaje 2 3 2 2" xfId="41"/>
+    <cellStyle name="Porcentaje 2 3 3" xfId="42"/>
+    <cellStyle name="Porcentaje 2 4" xfId="43"/>
+    <cellStyle name="Porcentaje 2 4 2" xfId="44"/>
+    <cellStyle name="Porcentaje 3" xfId="45"/>
+    <cellStyle name="Porcentaje 4" xfId="46"/>
+    <cellStyle name="Porcentaje 4 2" xfId="47"/>
+    <cellStyle name="Porcentaje 4 3" xfId="48"/>
+    <cellStyle name="Porcentaje 4 4" xfId="49"/>
+    <cellStyle name="Porcentaje 4 4 2" xfId="50"/>
+    <cellStyle name="Porcentaje 4 4 2 2" xfId="51"/>
+    <cellStyle name="Porcentaje 4 4 3" xfId="52"/>
+    <cellStyle name="Porcentaje 4 5" xfId="53"/>
+    <cellStyle name="Porcentaje 4 5 2" xfId="54"/>
+    <cellStyle name="Porcentaje 5" xfId="55"/>
+    <cellStyle name="Porcentaje 5 2" xfId="56"/>
+    <cellStyle name="Porcentaje 5 2 2" xfId="57"/>
+    <cellStyle name="Porcentaje 5 3" xfId="58"/>
+    <cellStyle name="Porcentaje 6" xfId="59"/>
+    <cellStyle name="Porcentaje 6 2" xfId="60"/>
+    <cellStyle name="Porcentaje 7" xfId="61"/>
+    <cellStyle name="Porcentaje 7 2" xfId="62"/>
   </cellStyles>
   <dxfs count="20">
     <dxf>
@@ -881,7 +1065,7 @@
   <dimension ref="A1:Q137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -989,11 +1173,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="191.25" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>

</xml_diff>

<commit_message>
Evaluación P2 y comentarios P32
</commit_message>
<xml_diff>
--- a/Evaluacion.xlsx
+++ b/Evaluacion.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Estudiante</t>
   </si>
@@ -128,6 +128,12 @@
       <t xml:space="preserve">. </t>
     </r>
   </si>
+  <si>
+    <t>Métodos ordenación implementados correctamente. RapidoFatal no explica la complejidad final, ni porqué se produce el stackoverflow. Tablas y gráficas correctos, especificando repeticiones. Cuidado al cambiar de número de repeticiones. No debería haber esas variaciones. Recuerda que las prácticas son individuales.</t>
+  </si>
+  <si>
+    <t>Antes de la entrega. Ni una línea implementada en github.</t>
+  </si>
 </sst>
 </file>
 
@@ -136,10 +142,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -311,73 +324,95 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -401,17 +436,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -420,13 +455,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -435,14 +470,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="107">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Hipervínculo 2" xfId="3"/>
     <cellStyle name="Hipervínculo 3" xfId="4"/>
@@ -463,44 +504,66 @@
     <cellStyle name="Normal 4 2 2 2" xfId="18"/>
     <cellStyle name="Normal 4 2 2 2 2" xfId="19"/>
     <cellStyle name="Normal 4 2 2 2 2 2" xfId="67"/>
+    <cellStyle name="Normal 4 2 2 2 2 3" xfId="89"/>
     <cellStyle name="Normal 4 2 2 2 3" xfId="66"/>
+    <cellStyle name="Normal 4 2 2 2 4" xfId="88"/>
     <cellStyle name="Normal 4 2 2 3" xfId="20"/>
     <cellStyle name="Normal 4 2 2 3 2" xfId="68"/>
+    <cellStyle name="Normal 4 2 2 3 3" xfId="90"/>
     <cellStyle name="Normal 4 2 2 4" xfId="65"/>
+    <cellStyle name="Normal 4 2 2 5" xfId="87"/>
     <cellStyle name="Normal 4 2 3" xfId="21"/>
     <cellStyle name="Normal 4 2 3 2" xfId="22"/>
     <cellStyle name="Normal 4 2 3 2 2" xfId="70"/>
+    <cellStyle name="Normal 4 2 3 2 3" xfId="92"/>
     <cellStyle name="Normal 4 2 3 3" xfId="69"/>
+    <cellStyle name="Normal 4 2 3 4" xfId="91"/>
     <cellStyle name="Normal 4 2 4" xfId="23"/>
     <cellStyle name="Normal 4 2 4 2" xfId="71"/>
+    <cellStyle name="Normal 4 2 4 3" xfId="93"/>
     <cellStyle name="Normal 4 2 5" xfId="64"/>
+    <cellStyle name="Normal 4 2 6" xfId="86"/>
     <cellStyle name="Normal 4 3" xfId="24"/>
     <cellStyle name="Normal 4 3 2" xfId="25"/>
     <cellStyle name="Normal 4 3 2 2" xfId="26"/>
     <cellStyle name="Normal 4 3 2 2 2" xfId="74"/>
+    <cellStyle name="Normal 4 3 2 2 3" xfId="96"/>
     <cellStyle name="Normal 4 3 2 3" xfId="73"/>
+    <cellStyle name="Normal 4 3 2 4" xfId="95"/>
     <cellStyle name="Normal 4 3 3" xfId="27"/>
     <cellStyle name="Normal 4 3 3 2" xfId="28"/>
     <cellStyle name="Normal 4 3 3 2 2" xfId="76"/>
+    <cellStyle name="Normal 4 3 3 2 3" xfId="98"/>
     <cellStyle name="Normal 4 3 3 3" xfId="75"/>
+    <cellStyle name="Normal 4 3 3 4" xfId="97"/>
     <cellStyle name="Normal 4 3 4" xfId="29"/>
     <cellStyle name="Normal 4 3 4 2" xfId="77"/>
+    <cellStyle name="Normal 4 3 4 3" xfId="99"/>
     <cellStyle name="Normal 4 3 5" xfId="72"/>
+    <cellStyle name="Normal 4 3 6" xfId="94"/>
     <cellStyle name="Normal 4 4" xfId="30"/>
     <cellStyle name="Normal 4 4 2" xfId="31"/>
     <cellStyle name="Normal 4 4 2 2" xfId="32"/>
     <cellStyle name="Normal 4 4 2 2 2" xfId="80"/>
+    <cellStyle name="Normal 4 4 2 2 3" xfId="102"/>
     <cellStyle name="Normal 4 4 2 3" xfId="79"/>
+    <cellStyle name="Normal 4 4 2 4" xfId="101"/>
     <cellStyle name="Normal 4 4 3" xfId="33"/>
     <cellStyle name="Normal 4 4 3 2" xfId="81"/>
+    <cellStyle name="Normal 4 4 3 3" xfId="103"/>
     <cellStyle name="Normal 4 4 4" xfId="78"/>
+    <cellStyle name="Normal 4 4 5" xfId="100"/>
     <cellStyle name="Normal 4 5" xfId="34"/>
     <cellStyle name="Normal 4 5 2" xfId="35"/>
     <cellStyle name="Normal 4 5 2 2" xfId="83"/>
+    <cellStyle name="Normal 4 5 2 3" xfId="105"/>
     <cellStyle name="Normal 4 5 3" xfId="82"/>
+    <cellStyle name="Normal 4 5 4" xfId="104"/>
     <cellStyle name="Normal 4 6" xfId="36"/>
     <cellStyle name="Normal 4 6 2" xfId="84"/>
+    <cellStyle name="Normal 4 6 3" xfId="106"/>
     <cellStyle name="Normal 4 7" xfId="63"/>
+    <cellStyle name="Normal 4 8" xfId="85"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
     <cellStyle name="Porcentaje 2" xfId="37"/>
     <cellStyle name="Porcentaje 2 2" xfId="38"/>
@@ -1147,7 +1210,7 @@
   <dimension ref="A1:Q137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+      <selection activeCell="D5" sqref="D5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1265,9 +1328,15 @@
       <c r="C5" s="16">
         <v>4</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="D5" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="17">
+        <v>8</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>

</xml_diff>